<commit_message>
updated boolean template and 14/03
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -349,8 +349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C512"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,7 +931,7 @@
         <v>0000110010</v>
       </c>
       <c r="C51" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -943,7 +943,7 @@
         <v>0000110011</v>
       </c>
       <c r="C52" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added 16/03 and updated boolean template
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -24,12 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="2">
+  <si>
+    <t>yes</t>
+  </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -349,8 +349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C512"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -475,7 +475,7 @@
         <v>0000001100</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -487,7 +487,7 @@
         <v>0000001101</v>
       </c>
       <c r="C14" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -499,7 +499,7 @@
         <v>0000001110</v>
       </c>
       <c r="C15" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -511,7 +511,7 @@
         <v>0000001111</v>
       </c>
       <c r="C16" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -523,7 +523,7 @@
         <v>0000010000</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -535,7 +535,7 @@
         <v>0000010001</v>
       </c>
       <c r="C18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,7 +547,7 @@
         <v>0000010010</v>
       </c>
       <c r="C19" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -559,7 +559,7 @@
         <v>0000010011</v>
       </c>
       <c r="C20" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -571,7 +571,7 @@
         <v>0000010100</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -583,7 +583,7 @@
         <v>0000010101</v>
       </c>
       <c r="C22" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -595,7 +595,7 @@
         <v>0000010110</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -607,7 +607,7 @@
         <v>0000010111</v>
       </c>
       <c r="C24" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -619,7 +619,7 @@
         <v>0000011000</v>
       </c>
       <c r="C25" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,7 +631,7 @@
         <v>0000011001</v>
       </c>
       <c r="C26" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -643,7 +643,7 @@
         <v>0000011010</v>
       </c>
       <c r="C27" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -655,7 +655,7 @@
         <v>0000011011</v>
       </c>
       <c r="C28" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>0000011100</v>
       </c>
       <c r="C29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -679,7 +679,7 @@
         <v>0000011101</v>
       </c>
       <c r="C30" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -691,7 +691,7 @@
         <v>0000011110</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
         <v>0000011111</v>
       </c>
       <c r="C32" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -715,7 +715,7 @@
         <v>0000100000</v>
       </c>
       <c r="C33" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -727,7 +727,7 @@
         <v>0000100001</v>
       </c>
       <c r="C34" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
         <v>0000100010</v>
       </c>
       <c r="C35" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,7 +751,7 @@
         <v>0000100011</v>
       </c>
       <c r="C36" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -763,7 +763,7 @@
         <v>0000100100</v>
       </c>
       <c r="C37" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -775,7 +775,7 @@
         <v>0000100101</v>
       </c>
       <c r="C38" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>0000100110</v>
       </c>
       <c r="C39" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -799,7 +799,7 @@
         <v>0000100111</v>
       </c>
       <c r="C40" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -811,7 +811,7 @@
         <v>0000101000</v>
       </c>
       <c r="C41" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -823,7 +823,7 @@
         <v>0000101001</v>
       </c>
       <c r="C42" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -835,7 +835,7 @@
         <v>0000101010</v>
       </c>
       <c r="C43" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -847,7 +847,7 @@
         <v>0000101011</v>
       </c>
       <c r="C44" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>0000101100</v>
       </c>
       <c r="C45" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -871,7 +871,7 @@
         <v>0000101101</v>
       </c>
       <c r="C46" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -883,7 +883,7 @@
         <v>0000101110</v>
       </c>
       <c r="C47" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -895,7 +895,7 @@
         <v>0000101111</v>
       </c>
       <c r="C48" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -907,7 +907,7 @@
         <v>0000110000</v>
       </c>
       <c r="C49" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -919,7 +919,7 @@
         <v>0000110001</v>
       </c>
       <c r="C50" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -931,7 +931,7 @@
         <v>0000110010</v>
       </c>
       <c r="C51" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -943,7 +943,7 @@
         <v>0000110011</v>
       </c>
       <c r="C52" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -967,7 +967,7 @@
         <v>0000110101</v>
       </c>
       <c r="C54" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -991,7 +991,7 @@
         <v>0000110111</v>
       </c>
       <c r="C56" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -1003,7 +1003,7 @@
         <v>0000111000</v>
       </c>
       <c r="C57" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1039,7 +1039,7 @@
         <v>0000111011</v>
       </c>
       <c r="C60" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -1063,7 +1063,7 @@
         <v>0000111101</v>
       </c>
       <c r="C62" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -1075,7 +1075,7 @@
         <v>0000111110</v>
       </c>
       <c r="C63" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -1087,7 +1087,7 @@
         <v>0000111111</v>
       </c>
       <c r="C64" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -1099,7 +1099,7 @@
         <v>0001000000</v>
       </c>
       <c r="C65" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -1111,7 +1111,7 @@
         <v>0001000001</v>
       </c>
       <c r="C66" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -1218,6 +1218,9 @@
         <f t="shared" si="1"/>
         <v>0001001010</v>
       </c>
+      <c r="C75" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76">
@@ -1227,6 +1230,9 @@
         <f t="shared" si="1"/>
         <v>0001001011</v>
       </c>
+      <c r="C76" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77">
@@ -1236,6 +1242,9 @@
         <f t="shared" si="1"/>
         <v>0001001100</v>
       </c>
+      <c r="C77" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78">
@@ -1245,6 +1254,9 @@
         <f t="shared" si="1"/>
         <v>0001001101</v>
       </c>
+      <c r="C78" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79">
@@ -1254,6 +1266,9 @@
         <f t="shared" si="1"/>
         <v>0001001110</v>
       </c>
+      <c r="C79" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80">
@@ -1263,8 +1278,11 @@
         <f t="shared" si="1"/>
         <v>0001001111</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1272,8 +1290,11 @@
         <f t="shared" si="1"/>
         <v>0001010000</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1281,8 +1302,11 @@
         <f t="shared" si="1"/>
         <v>0001010001</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1290,8 +1314,11 @@
         <f t="shared" si="1"/>
         <v>0001010010</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1299,8 +1326,11 @@
         <f t="shared" si="1"/>
         <v>0001010011</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1308,8 +1338,11 @@
         <f t="shared" si="1"/>
         <v>0001010100</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1317,8 +1350,11 @@
         <f t="shared" si="1"/>
         <v>0001010101</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1326,8 +1362,11 @@
         <f t="shared" si="1"/>
         <v>0001010110</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1335,8 +1374,11 @@
         <f t="shared" si="1"/>
         <v>0001010111</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1344,8 +1386,11 @@
         <f t="shared" si="1"/>
         <v>0001011000</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -1353,8 +1398,11 @@
         <f t="shared" si="1"/>
         <v>0001011001</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -1363,7 +1411,7 @@
         <v>0001011010</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>91</v>
       </c>
@@ -1372,7 +1420,7 @@
         <v>0001011011</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>92</v>
       </c>
@@ -1381,7 +1429,7 @@
         <v>0001011100</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>93</v>
       </c>
@@ -1390,7 +1438,7 @@
         <v>0001011101</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>94</v>
       </c>
@@ -1399,7 +1447,7 @@
         <v>0001011110</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>95</v>
       </c>
@@ -1552,7 +1600,7 @@
         <v>0001101111</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>112</v>
       </c>
@@ -1561,7 +1609,7 @@
         <v>0001110000</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>113</v>
       </c>
@@ -1570,7 +1618,7 @@
         <v>0001110001</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>114</v>
       </c>
@@ -1579,7 +1627,7 @@
         <v>0001110010</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>115</v>
       </c>
@@ -1588,7 +1636,7 @@
         <v>0001110011</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>116</v>
       </c>
@@ -1597,7 +1645,7 @@
         <v>0001110100</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>117</v>
       </c>
@@ -1606,7 +1654,7 @@
         <v>0001110101</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>118</v>
       </c>
@@ -1615,7 +1663,7 @@
         <v>0001110110</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>119</v>
       </c>
@@ -1624,7 +1672,7 @@
         <v>0001110111</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>120</v>
       </c>
@@ -1633,7 +1681,7 @@
         <v>0001111000</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>121</v>
       </c>
@@ -1642,7 +1690,7 @@
         <v>0001111001</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>122</v>
       </c>
@@ -1651,7 +1699,7 @@
         <v>0001111010</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>123</v>
       </c>
@@ -1660,7 +1708,7 @@
         <v>0001111011</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>124</v>
       </c>
@@ -1669,7 +1717,7 @@
         <v>0001111100</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>125</v>
       </c>
@@ -1678,7 +1726,7 @@
         <v>0001111101</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>126</v>
       </c>
@@ -1687,13 +1735,16 @@
         <v>0001111110</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>127</v>
       </c>
       <c r="B128" t="str">
         <f t="shared" si="1"/>
         <v>0001111111</v>
+      </c>
+      <c r="C128" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
@@ -2704,7 +2755,7 @@
         <v>0011101111</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>240</v>
       </c>
@@ -2713,7 +2764,7 @@
         <v>0011110000</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>241</v>
       </c>
@@ -2722,7 +2773,7 @@
         <v>0011110001</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>242</v>
       </c>
@@ -2731,7 +2782,7 @@
         <v>0011110010</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>243</v>
       </c>
@@ -2740,7 +2791,7 @@
         <v>0011110011</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>244</v>
       </c>
@@ -2749,7 +2800,7 @@
         <v>0011110100</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>245</v>
       </c>
@@ -2758,7 +2809,7 @@
         <v>0011110101</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>246</v>
       </c>
@@ -2767,7 +2818,7 @@
         <v>0011110110</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>247</v>
       </c>
@@ -2776,7 +2827,7 @@
         <v>0011110111</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>248</v>
       </c>
@@ -2785,7 +2836,7 @@
         <v>0011111000</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>249</v>
       </c>
@@ -2794,7 +2845,7 @@
         <v>0011111001</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>250</v>
       </c>
@@ -2803,7 +2854,7 @@
         <v>0011111010</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>251</v>
       </c>
@@ -2812,7 +2863,7 @@
         <v>0011111011</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>252</v>
       </c>
@@ -2821,7 +2872,7 @@
         <v>0011111100</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>253</v>
       </c>
@@ -2830,7 +2881,7 @@
         <v>0011111101</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>254</v>
       </c>
@@ -2839,13 +2890,16 @@
         <v>0011111110</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>255</v>
       </c>
       <c r="B256" t="str">
         <f t="shared" si="3"/>
         <v>0011111111</v>
+      </c>
+      <c r="C256" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.25">
@@ -5008,7 +5062,7 @@
         <v>0111101111</v>
       </c>
     </row>
-    <row r="497" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A497">
         <v>496</v>
       </c>
@@ -5017,7 +5071,7 @@
         <v>0111110000</v>
       </c>
     </row>
-    <row r="498" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A498">
         <v>497</v>
       </c>
@@ -5026,7 +5080,7 @@
         <v>0111110001</v>
       </c>
     </row>
-    <row r="499" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A499">
         <v>498</v>
       </c>
@@ -5035,7 +5089,7 @@
         <v>0111110010</v>
       </c>
     </row>
-    <row r="500" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A500">
         <v>499</v>
       </c>
@@ -5044,7 +5098,7 @@
         <v>0111110011</v>
       </c>
     </row>
-    <row r="501" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="501" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A501">
         <v>500</v>
       </c>
@@ -5053,7 +5107,7 @@
         <v>0111110100</v>
       </c>
     </row>
-    <row r="502" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A502">
         <v>501</v>
       </c>
@@ -5062,7 +5116,7 @@
         <v>0111110101</v>
       </c>
     </row>
-    <row r="503" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="503" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A503">
         <v>502</v>
       </c>
@@ -5071,7 +5125,7 @@
         <v>0111110110</v>
       </c>
     </row>
-    <row r="504" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="504" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A504">
         <v>503</v>
       </c>
@@ -5080,7 +5134,7 @@
         <v>0111110111</v>
       </c>
     </row>
-    <row r="505" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="505" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A505">
         <v>504</v>
       </c>
@@ -5089,7 +5143,7 @@
         <v>0111111000</v>
       </c>
     </row>
-    <row r="506" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A506">
         <v>505</v>
       </c>
@@ -5098,7 +5152,7 @@
         <v>0111111001</v>
       </c>
     </row>
-    <row r="507" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A507">
         <v>506</v>
       </c>
@@ -5107,7 +5161,7 @@
         <v>0111111010</v>
       </c>
     </row>
-    <row r="508" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A508">
         <v>507</v>
       </c>
@@ -5116,7 +5170,7 @@
         <v>0111111011</v>
       </c>
     </row>
-    <row r="509" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A509">
         <v>508</v>
       </c>
@@ -5125,7 +5179,7 @@
         <v>0111111100</v>
       </c>
     </row>
-    <row r="510" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="510" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A510">
         <v>509</v>
       </c>
@@ -5134,7 +5188,7 @@
         <v>0111111101</v>
       </c>
     </row>
-    <row r="511" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A511">
         <v>510</v>
       </c>
@@ -5143,13 +5197,16 @@
         <v>0111111110</v>
       </c>
     </row>
-    <row r="512" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="512" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A512">
         <v>511</v>
       </c>
       <c r="B512" t="str">
         <f t="shared" si="7"/>
         <v>0111111111</v>
+      </c>
+      <c r="C512" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>